<commit_message>
Må tweakes mer disse bedward capacitiene...
</commit_message>
<xml_diff>
--- a/input_output/results.xlsx
+++ b/input_output/results.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BR31"/>
+  <dimension ref="A1:BR47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
@@ -4525,6 +4525,2913 @@
         <v>0</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>9</v>
+      </c>
+      <c r="B32" t="n">
+        <v>60</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3931.833333333332</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3657.628549937135</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.06973967616367184</v>
+      </c>
+      <c r="H32" t="n">
+        <v>60.03021001815796</v>
+      </c>
+      <c r="I32" t="n">
+        <v>60</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>TIME_LIMIT</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>24.4161779535326</v>
+      </c>
+      <c r="N32" t="n">
+        <v>29.14713234663655</v>
+      </c>
+      <c r="O32" t="n">
+        <v>29.29083753609626</v>
+      </c>
+      <c r="P32" t="n">
+        <v>28.77040362183271</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>24.23002945261412</v>
+      </c>
+      <c r="R32" t="n">
+        <v>18.05576797517152</v>
+      </c>
+      <c r="S32" t="n">
+        <v>14.02379333154378</v>
+      </c>
+      <c r="T32" t="n">
+        <v>23.52673233872696</v>
+      </c>
+      <c r="U32" t="n">
+        <v>27.07405007955554</v>
+      </c>
+      <c r="V32" t="n">
+        <v>27.83102102629444</v>
+      </c>
+      <c r="W32" t="n">
+        <v>27.25032531805808</v>
+      </c>
+      <c r="X32" t="n">
+        <v>24.17222124478874</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>18.08523631800681</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>14.02082007615748</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>21.14409060090202</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>27.00170470698584</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>28.08381482591541</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>28.40475424346277</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>24.23331480605033</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>17.94508930995797</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>13.89156104941151</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>23.53191932010482</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>27.3127593904627</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>28.03606840417485</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>28.09594866280807</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>24.1801415893659</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>18.41604138353239</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>14.585691092529</v>
+      </c>
+      <c r="AO32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ32" t="n">
+        <v>4.286011277056029</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>5.0113674912858</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>4.625904440981075</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>4.186064132621791</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>2.809357456526018</v>
+      </c>
+      <c r="AV32" t="n">
+        <v>0.7969668716547034</v>
+      </c>
+      <c r="AW32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX32" t="n">
+        <v>4.757862318309479</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>5.084562464129603</v>
+      </c>
+      <c r="AZ32" t="n">
+        <v>4.821861547077239</v>
+      </c>
+      <c r="BA32" t="n">
+        <v>4.165843496495312</v>
+      </c>
+      <c r="BB32" t="n">
+        <v>2.844105610760583</v>
+      </c>
+      <c r="BC32" t="n">
+        <v>0.8600764333515295</v>
+      </c>
+      <c r="BD32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE32" t="n">
+        <v>4.99362322949111</v>
+      </c>
+      <c r="BF32" t="n">
+        <v>5.302522946272227</v>
+      </c>
+      <c r="BG32" t="n">
+        <v>4.727993342031557</v>
+      </c>
+      <c r="BH32" t="n">
+        <v>4.244917421799359</v>
+      </c>
+      <c r="BI32" t="n">
+        <v>2.845043601952899</v>
+      </c>
+      <c r="BJ32" t="n">
+        <v>0.8192880093152936</v>
+      </c>
+      <c r="BK32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL32" t="n">
+        <v>4.759038212394366</v>
+      </c>
+      <c r="BM32" t="n">
+        <v>5.28177229530379</v>
+      </c>
+      <c r="BN32" t="n">
+        <v>4.996929228254876</v>
+      </c>
+      <c r="BO32" t="n">
+        <v>4.896346788931567</v>
+      </c>
+      <c r="BP32" t="n">
+        <v>2.895022300413254</v>
+      </c>
+      <c r="BQ32" t="n">
+        <v>0.6695843527103001</v>
+      </c>
+      <c r="BR32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>------------------- Begin Heuristic -------------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>9</v>
+      </c>
+      <c r="B34" t="n">
+        <v>60</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3960.8416653109</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3731.613873315454</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.05787350552359243</v>
+      </c>
+      <c r="H34" t="n">
+        <v>60.02555584907532</v>
+      </c>
+      <c r="I34" t="n">
+        <v>10</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>TIME_LIMIT</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>24.28520849296931</v>
+      </c>
+      <c r="N34" t="n">
+        <v>28.98480556591142</v>
+      </c>
+      <c r="O34" t="n">
+        <v>29.12092626984135</v>
+      </c>
+      <c r="P34" t="n">
+        <v>28.64571969697145</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>24.31602021529559</v>
+      </c>
+      <c r="R34" t="n">
+        <v>18.15603399829669</v>
+      </c>
+      <c r="S34" t="n">
+        <v>14.05513863095996</v>
+      </c>
+      <c r="T34" t="n">
+        <v>23.57807408233832</v>
+      </c>
+      <c r="U34" t="n">
+        <v>27.10527386906098</v>
+      </c>
+      <c r="V34" t="n">
+        <v>27.72250454949679</v>
+      </c>
+      <c r="W34" t="n">
+        <v>27.29553938785307</v>
+      </c>
+      <c r="X34" t="n">
+        <v>24.35545765685573</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>18.06645522588815</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>13.85854017706021</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>21.06284090842615</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>26.85689123880027</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>27.85824156113372</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>28.28314926580282</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>24.23823621461629</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>18.01915986757706</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>13.88312919191032</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>23.4953488394262</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>27.2932072152042</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>28.01798849138331</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>28.10405149880267</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>24.24779900078737</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>18.47205082152544</v>
+      </c>
+      <c r="AN34" t="n">
+        <v>14.60543394890114</v>
+      </c>
+      <c r="AO34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ34" t="n">
+        <v>4.274725284830357</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>4.976267272699181</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>4.644187101294957</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>4.251766167306537</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>2.821311568793756</v>
+      </c>
+      <c r="AV34" t="n">
+        <v>0.7825788691398882</v>
+      </c>
+      <c r="AW34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX34" t="n">
+        <v>4.796231414070542</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>5.092589951278025</v>
+      </c>
+      <c r="AZ34" t="n">
+        <v>4.786452341006744</v>
+      </c>
+      <c r="BA34" t="n">
+        <v>3.927837966493114</v>
+      </c>
+      <c r="BB34" t="n">
+        <v>2.80739130887253</v>
+      </c>
+      <c r="BC34" t="n">
+        <v>0.9087219053104476</v>
+      </c>
+      <c r="BD34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE34" t="n">
+        <v>5.018304904500121</v>
+      </c>
+      <c r="BF34" t="n">
+        <v>5.295881837598918</v>
+      </c>
+      <c r="BG34" t="n">
+        <v>4.712393390024335</v>
+      </c>
+      <c r="BH34" t="n">
+        <v>4.475614234932291</v>
+      </c>
+      <c r="BI34" t="n">
+        <v>2.826134263054751</v>
+      </c>
+      <c r="BJ34" t="n">
+        <v>0.7361131092962193</v>
+      </c>
+      <c r="BK34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL34" t="n">
+        <v>4.838870595794765</v>
+      </c>
+      <c r="BM34" t="n">
+        <v>5.304396515407181</v>
+      </c>
+      <c r="BN34" t="n">
+        <v>5.016391300073019</v>
+      </c>
+      <c r="BO34" t="n">
+        <v>4.867274688974495</v>
+      </c>
+      <c r="BP34" t="n">
+        <v>2.877957758929822</v>
+      </c>
+      <c r="BQ34" t="n">
+        <v>0.6714808118834654</v>
+      </c>
+      <c r="BR34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>9</v>
+      </c>
+      <c r="B35" t="n">
+        <v>60</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4175.662499149959</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3920.945595501683</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.06100035711701527</v>
+      </c>
+      <c r="H35" t="n">
+        <v>60.02707695960999</v>
+      </c>
+      <c r="I35" t="n">
+        <v>10</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>TIME_LIMIT</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>24.36236633011488</v>
+      </c>
+      <c r="N35" t="n">
+        <v>29.05399108051006</v>
+      </c>
+      <c r="O35" t="n">
+        <v>29.21806605425384</v>
+      </c>
+      <c r="P35" t="n">
+        <v>28.72120688522326</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>24.30579825433666</v>
+      </c>
+      <c r="R35" t="n">
+        <v>17.95515344173036</v>
+      </c>
+      <c r="S35" t="n">
+        <v>13.86232517021557</v>
+      </c>
+      <c r="T35" t="n">
+        <v>23.41458628751112</v>
+      </c>
+      <c r="U35" t="n">
+        <v>27.06374430147042</v>
+      </c>
+      <c r="V35" t="n">
+        <v>27.09008844358921</v>
+      </c>
+      <c r="W35" t="n">
+        <v>26.26955971750057</v>
+      </c>
+      <c r="X35" t="n">
+        <v>24.23443796648827</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>18.07165861925771</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>13.96570791284627</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>21.15410192461368</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>26.87512736564382</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>27.86540622215237</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>28.29744046106617</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>24.22433006507573</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>17.81484837754029</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>13.7691825105021</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>23.44069887659263</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>27.30894325306893</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>27.62490699550615</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>27.29986996561677</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>24.25558819941221</v>
+      </c>
+      <c r="AM35" t="n">
+        <v>18.38906280560153</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>14.51204842597451</v>
+      </c>
+      <c r="AO35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ35" t="n">
+        <v>4.232204123346179</v>
+      </c>
+      <c r="AR35" t="n">
+        <v>4.980535811683633</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>4.451912484171198</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>3.974330622207145</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>2.828381419503939</v>
+      </c>
+      <c r="AV35" t="n">
+        <v>0.8406599165019686</v>
+      </c>
+      <c r="AW35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX35" t="n">
+        <v>4.789441849593182</v>
+      </c>
+      <c r="AY35" t="n">
+        <v>5.076029947594361</v>
+      </c>
+      <c r="AZ35" t="n">
+        <v>4.824014578297528</v>
+      </c>
+      <c r="BA35" t="n">
+        <v>4.040524653005679</v>
+      </c>
+      <c r="BB35" t="n">
+        <v>2.791776289633468</v>
+      </c>
+      <c r="BC35" t="n">
+        <v>0.8616715537666075</v>
+      </c>
+      <c r="BD35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE35" t="n">
+        <v>4.891894037996959</v>
+      </c>
+      <c r="BF35" t="n">
+        <v>5.213884193248749</v>
+      </c>
+      <c r="BG35" t="n">
+        <v>4.631343054359643</v>
+      </c>
+      <c r="BH35" t="n">
+        <v>4.26855916972442</v>
+      </c>
+      <c r="BI35" t="n">
+        <v>2.850589963551472</v>
+      </c>
+      <c r="BJ35" t="n">
+        <v>0.810558507519298</v>
+      </c>
+      <c r="BK35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL35" t="n">
+        <v>4.823302810016049</v>
+      </c>
+      <c r="BM35" t="n">
+        <v>5.278240368396812</v>
+      </c>
+      <c r="BN35" t="n">
+        <v>5.04810051380056</v>
+      </c>
+      <c r="BO35" t="n">
+        <v>4.693214083786344</v>
+      </c>
+      <c r="BP35" t="n">
+        <v>2.864909147389509</v>
+      </c>
+      <c r="BQ35" t="n">
+        <v>0.7196151858000375</v>
+      </c>
+      <c r="BR35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>4</v>
+      </c>
+      <c r="B36" t="n">
+        <v>60</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1082.05</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1082.05</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>3.243115901947021</v>
+      </c>
+      <c r="I36" t="n">
+        <v>600</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>12.3434044081845</v>
+      </c>
+      <c r="N36" t="n">
+        <v>13.5202253280347</v>
+      </c>
+      <c r="O36" t="n">
+        <v>14.61611339358766</v>
+      </c>
+      <c r="P36" t="n">
+        <v>14.8158117085236</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>15.33537460404402</v>
+      </c>
+      <c r="R36" t="n">
+        <v>12.51314774103081</v>
+      </c>
+      <c r="S36" t="n">
+        <v>10.24905377592563</v>
+      </c>
+      <c r="T36" t="n">
+        <v>11.73536728856415</v>
+      </c>
+      <c r="U36" t="n">
+        <v>12.96776932434242</v>
+      </c>
+      <c r="V36" t="n">
+        <v>14.04403534636135</v>
+      </c>
+      <c r="W36" t="n">
+        <v>14.57903832824672</v>
+      </c>
+      <c r="X36" t="n">
+        <v>14.93286999951201</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>12.60038424884078</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>10.48662947841608</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>11.39400962907285</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>12.62885908836435</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>13.75773540819628</v>
+      </c>
+      <c r="AD36" t="n">
+        <v>14.12858740628091</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>14.85196578027257</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>12.19415736188307</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>10.01633500162759</v>
+      </c>
+      <c r="AH36" t="n">
+        <v>11.53692568249016</v>
+      </c>
+      <c r="AI36" t="n">
+        <v>12.75777726004549</v>
+      </c>
+      <c r="AJ36" t="n">
+        <v>13.92920546965477</v>
+      </c>
+      <c r="AK36" t="n">
+        <v>14.67391375308276</v>
+      </c>
+      <c r="AL36" t="n">
+        <v>15.02554216524064</v>
+      </c>
+      <c r="AM36" t="n">
+        <v>12.54519553061307</v>
+      </c>
+      <c r="AN36" t="n">
+        <v>10.3672606877251</v>
+      </c>
+      <c r="AO36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ36" t="n">
+        <v>1.864768336839937</v>
+      </c>
+      <c r="AR36" t="n">
+        <v>3.229642212778394</v>
+      </c>
+      <c r="AS36" t="n">
+        <v>3.266125512194973</v>
+      </c>
+      <c r="AT36" t="n">
+        <v>2.654811168399731</v>
+      </c>
+      <c r="AU36" t="n">
+        <v>1.981996286885576</v>
+      </c>
+      <c r="AV36" t="n">
+        <v>0.5538812192532928</v>
+      </c>
+      <c r="AW36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX36" t="n">
+        <v>2.48165831688145</v>
+      </c>
+      <c r="AY36" t="n">
+        <v>3.748299474598488</v>
+      </c>
+      <c r="AZ36" t="n">
+        <v>3.601694627062064</v>
+      </c>
+      <c r="BA36" t="n">
+        <v>2.667941231873567</v>
+      </c>
+      <c r="BB36" t="n">
+        <v>1.98899409747194</v>
+      </c>
+      <c r="BC36" t="n">
+        <v>0.6282727382934157</v>
+      </c>
+      <c r="BD36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE36" t="n">
+        <v>1.81248276272409</v>
+      </c>
+      <c r="BF36" t="n">
+        <v>3.334804464407505</v>
+      </c>
+      <c r="BG36" t="n">
+        <v>3.35653663339991</v>
+      </c>
+      <c r="BH36" t="n">
+        <v>2.587824785011986</v>
+      </c>
+      <c r="BI36" t="n">
+        <v>2.000138783999859</v>
+      </c>
+      <c r="BJ36" t="n">
+        <v>0.5936333111581259</v>
+      </c>
+      <c r="BK36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL36" t="n">
+        <v>2.291553506914124</v>
+      </c>
+      <c r="BM36" t="n">
+        <v>3.719325909966189</v>
+      </c>
+      <c r="BN36" t="n">
+        <v>3.692806092148585</v>
+      </c>
+      <c r="BO36" t="n">
+        <v>2.595280175937613</v>
+      </c>
+      <c r="BP36" t="n">
+        <v>1.935398814642308</v>
+      </c>
+      <c r="BQ36" t="n">
+        <v>0.6274614659348009</v>
+      </c>
+      <c r="BR36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>------------------- Begin Heuristic -------------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>4</v>
+      </c>
+      <c r="B38" t="n">
+        <v>60</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1183.595833333333</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1183.595833333332</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>4.479067802429199</v>
+      </c>
+      <c r="I38" t="n">
+        <v>10</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>12.27936933591642</v>
+      </c>
+      <c r="N38" t="n">
+        <v>13.50488264561126</v>
+      </c>
+      <c r="O38" t="n">
+        <v>14.69965218468893</v>
+      </c>
+      <c r="P38" t="n">
+        <v>14.97023392910024</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>15.50735458393346</v>
+      </c>
+      <c r="R38" t="n">
+        <v>12.64256448654179</v>
+      </c>
+      <c r="S38" t="n">
+        <v>10.34648695190329</v>
+      </c>
+      <c r="T38" t="n">
+        <v>11.67815777841026</v>
+      </c>
+      <c r="U38" t="n">
+        <v>12.84861911322067</v>
+      </c>
+      <c r="V38" t="n">
+        <v>13.80006624072945</v>
+      </c>
+      <c r="W38" t="n">
+        <v>14.42848829193973</v>
+      </c>
+      <c r="X38" t="n">
+        <v>14.61292777808824</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>12.26111130317301</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>10.21540716165076</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>11.26603059334872</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>12.57986733249986</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>13.83978332549718</v>
+      </c>
+      <c r="AD38" t="n">
+        <v>14.25576029743573</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>15.17363940876898</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>12.47344276972833</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>10.22675632980433</v>
+      </c>
+      <c r="AH38" t="n">
+        <v>11.66100082656825</v>
+      </c>
+      <c r="AI38" t="n">
+        <v>12.86080021509062</v>
+      </c>
+      <c r="AJ38" t="n">
+        <v>13.86108212361502</v>
+      </c>
+      <c r="AK38" t="n">
+        <v>14.56204033349343</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>14.70606941191173</v>
+      </c>
+      <c r="AM38" t="n">
+        <v>12.1857300289383</v>
+      </c>
+      <c r="AN38" t="n">
+        <v>10.04009919200209</v>
+      </c>
+      <c r="AO38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ38" t="n">
+        <v>1.898220011146666</v>
+      </c>
+      <c r="AR38" t="n">
+        <v>3.280221523929653</v>
+      </c>
+      <c r="AS38" t="n">
+        <v>3.366154350025274</v>
+      </c>
+      <c r="AT38" t="n">
+        <v>2.64700219868854</v>
+      </c>
+      <c r="AU38" t="n">
+        <v>1.972951299066402</v>
+      </c>
+      <c r="AV38" t="n">
+        <v>0.5662819197943363</v>
+      </c>
+      <c r="AW38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX38" t="n">
+        <v>2.37323163694846</v>
+      </c>
+      <c r="AY38" t="n">
+        <v>3.637066256955228</v>
+      </c>
+      <c r="AZ38" t="n">
+        <v>3.454322379195133</v>
+      </c>
+      <c r="BA38" t="n">
+        <v>2.560221694209244</v>
+      </c>
+      <c r="BB38" t="n">
+        <v>1.939148938525835</v>
+      </c>
+      <c r="BC38" t="n">
+        <v>0.6268785596621577</v>
+      </c>
+      <c r="BD38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE38" t="n">
+        <v>1.949313865130213</v>
+      </c>
+      <c r="BF38" t="n">
+        <v>3.370326084284571</v>
+      </c>
+      <c r="BG38" t="n">
+        <v>3.508072961547001</v>
+      </c>
+      <c r="BH38" t="n">
+        <v>2.75874508159929</v>
+      </c>
+      <c r="BI38" t="n">
+        <v>1.99046698192744</v>
+      </c>
+      <c r="BJ38" t="n">
+        <v>0.559310022184544</v>
+      </c>
+      <c r="BK38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL38" t="n">
+        <v>2.408881522632248</v>
+      </c>
+      <c r="BM38" t="n">
+        <v>3.662707973133359</v>
+      </c>
+      <c r="BN38" t="n">
+        <v>3.330292110933521</v>
+      </c>
+      <c r="BO38" t="n">
+        <v>2.351144204291153</v>
+      </c>
+      <c r="BP38" t="n">
+        <v>1.906050147833227</v>
+      </c>
+      <c r="BQ38" t="n">
+        <v>0.6396538776864269</v>
+      </c>
+      <c r="BR38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" t="n">
+        <v>60</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1183.595833333333</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1183.595833333332</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3.846158027648926</v>
+      </c>
+      <c r="I39" t="n">
+        <v>10</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>12.34062976913913</v>
+      </c>
+      <c r="N39" t="n">
+        <v>13.49432818490398</v>
+      </c>
+      <c r="O39" t="n">
+        <v>14.67327655502846</v>
+      </c>
+      <c r="P39" t="n">
+        <v>14.81559095432781</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>15.42678518496122</v>
+      </c>
+      <c r="R39" t="n">
+        <v>12.60442499395258</v>
+      </c>
+      <c r="S39" t="n">
+        <v>10.33342949240147</v>
+      </c>
+      <c r="T39" t="n">
+        <v>11.67105864892298</v>
+      </c>
+      <c r="U39" t="n">
+        <v>12.87131369779762</v>
+      </c>
+      <c r="V39" t="n">
+        <v>13.95248804897131</v>
+      </c>
+      <c r="W39" t="n">
+        <v>14.63076571426144</v>
+      </c>
+      <c r="X39" t="n">
+        <v>14.94008828456298</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>12.53937529119693</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>10.42895771735566</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>11.33563049212768</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>12.57096779863304</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>13.92805941627175</v>
+      </c>
+      <c r="AD39" t="n">
+        <v>14.32840905663268</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>15.12231062736682</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>12.40432037699027</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>10.14383899759455</v>
+      </c>
+      <c r="AH39" t="n">
+        <v>11.56559070911058</v>
+      </c>
+      <c r="AI39" t="n">
+        <v>12.73000652971256</v>
+      </c>
+      <c r="AJ39" t="n">
+        <v>13.74063710882452</v>
+      </c>
+      <c r="AK39" t="n">
+        <v>14.39370566121094</v>
+      </c>
+      <c r="AL39" t="n">
+        <v>14.69834458969904</v>
+      </c>
+      <c r="AM39" t="n">
+        <v>12.16129193682339</v>
+      </c>
+      <c r="AN39" t="n">
+        <v>10.01133091872873</v>
+      </c>
+      <c r="AO39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ39" t="n">
+        <v>1.865627167115387</v>
+      </c>
+      <c r="AR39" t="n">
+        <v>3.31499954414534</v>
+      </c>
+      <c r="AS39" t="n">
+        <v>3.351021002339279</v>
+      </c>
+      <c r="AT39" t="n">
+        <v>2.679979544231284</v>
+      </c>
+      <c r="AU39" t="n">
+        <v>1.944481610991843</v>
+      </c>
+      <c r="AV39" t="n">
+        <v>0.5308155645575637</v>
+      </c>
+      <c r="AW39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX39" t="n">
+        <v>2.444243366366629</v>
+      </c>
+      <c r="AY39" t="n">
+        <v>3.751606440871917</v>
+      </c>
+      <c r="AZ39" t="n">
+        <v>3.481523400890596</v>
+      </c>
+      <c r="BA39" t="n">
+        <v>2.730861153718398</v>
+      </c>
+      <c r="BB39" t="n">
+        <v>1.947559496725652</v>
+      </c>
+      <c r="BC39" t="n">
+        <v>0.5647918746448369</v>
+      </c>
+      <c r="BD39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE39" t="n">
+        <v>1.91819724446512</v>
+      </c>
+      <c r="BF39" t="n">
+        <v>3.328820108461018</v>
+      </c>
+      <c r="BG39" t="n">
+        <v>3.474235928760088</v>
+      </c>
+      <c r="BH39" t="n">
+        <v>2.705276569173543</v>
+      </c>
+      <c r="BI39" t="n">
+        <v>1.972194399885293</v>
+      </c>
+      <c r="BJ39" t="n">
+        <v>0.5622022401076352</v>
+      </c>
+      <c r="BK39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL39" t="n">
+        <v>2.433478567197623</v>
+      </c>
+      <c r="BM39" t="n">
+        <v>3.516260844006164</v>
+      </c>
+      <c r="BN39" t="n">
+        <v>3.17950226700248</v>
+      </c>
+      <c r="BO39" t="n">
+        <v>2.637401742624237</v>
+      </c>
+      <c r="BP39" t="n">
+        <v>1.888782786359301</v>
+      </c>
+      <c r="BQ39" t="n">
+        <v>0.5328027366887004</v>
+      </c>
+      <c r="BR39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>4</v>
+      </c>
+      <c r="B40" t="n">
+        <v>60</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1183.595833333333</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1183.595833333332</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>4.122068166732788</v>
+      </c>
+      <c r="I40" t="n">
+        <v>10</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>12.34789959391541</v>
+      </c>
+      <c r="N40" t="n">
+        <v>13.54181613389421</v>
+      </c>
+      <c r="O40" t="n">
+        <v>14.6494250002446</v>
+      </c>
+      <c r="P40" t="n">
+        <v>14.92908296797663</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>15.44776438461672</v>
+      </c>
+      <c r="R40" t="n">
+        <v>12.56759618952965</v>
+      </c>
+      <c r="S40" t="n">
+        <v>10.27096968965916</v>
+      </c>
+      <c r="T40" t="n">
+        <v>11.61818606524989</v>
+      </c>
+      <c r="U40" t="n">
+        <v>12.68447856801594</v>
+      </c>
+      <c r="V40" t="n">
+        <v>13.73612670003582</v>
+      </c>
+      <c r="W40" t="n">
+        <v>14.29205098084066</v>
+      </c>
+      <c r="X40" t="n">
+        <v>14.60148203033945</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>12.27037936536802</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>10.18602341952079</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>11.21100417218991</v>
+      </c>
+      <c r="AB40" t="n">
+        <v>12.51772209447278</v>
+      </c>
+      <c r="AC40" t="n">
+        <v>13.84357703437443</v>
+      </c>
+      <c r="AD40" t="n">
+        <v>14.32406510416142</v>
+      </c>
+      <c r="AE40" t="n">
+        <v>15.15027759018553</v>
+      </c>
+      <c r="AF40" t="n">
+        <v>12.47814680844429</v>
+      </c>
+      <c r="AG40" t="n">
+        <v>10.27833481857003</v>
+      </c>
+      <c r="AH40" t="n">
+        <v>11.73519721410645</v>
+      </c>
+      <c r="AI40" t="n">
+        <v>12.71416046491356</v>
+      </c>
+      <c r="AJ40" t="n">
+        <v>13.72814372282082</v>
+      </c>
+      <c r="AK40" t="n">
+        <v>14.41466794545817</v>
+      </c>
+      <c r="AL40" t="n">
+        <v>14.90386023641348</v>
+      </c>
+      <c r="AM40" t="n">
+        <v>12.41832547660643</v>
+      </c>
+      <c r="AN40" t="n">
+        <v>10.24371752364071</v>
+      </c>
+      <c r="AO40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ40" t="n">
+        <v>1.853020102841077</v>
+      </c>
+      <c r="AR40" t="n">
+        <v>3.274589363976532</v>
+      </c>
+      <c r="AS40" t="n">
+        <v>3.288012317588266</v>
+      </c>
+      <c r="AT40" t="n">
+        <v>2.661318621927861</v>
+      </c>
+      <c r="AU40" t="n">
+        <v>1.962317745874309</v>
+      </c>
+      <c r="AV40" t="n">
+        <v>0.5387588240851421</v>
+      </c>
+      <c r="AW40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX40" t="n">
+        <v>2.385223374096777</v>
+      </c>
+      <c r="AY40" t="n">
+        <v>3.419058349338067</v>
+      </c>
+      <c r="AZ40" t="n">
+        <v>3.489344680152869</v>
+      </c>
+      <c r="BA40" t="n">
+        <v>2.687801318511028</v>
+      </c>
+      <c r="BB40" t="n">
+        <v>1.925514145397006</v>
+      </c>
+      <c r="BC40" t="n">
+        <v>0.58686135749617</v>
+      </c>
+      <c r="BD40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE40" t="n">
+        <v>2.011259039509975</v>
+      </c>
+      <c r="BF40" t="n">
+        <v>3.438708294472476</v>
+      </c>
+      <c r="BG40" t="n">
+        <v>3.585582620991028</v>
+      </c>
+      <c r="BH40" t="n">
+        <v>2.698011537786374</v>
+      </c>
+      <c r="BI40" t="n">
+        <v>1.982206627305143</v>
+      </c>
+      <c r="BJ40" t="n">
+        <v>0.5878491358935091</v>
+      </c>
+      <c r="BK40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL40" t="n">
+        <v>2.434552163249291</v>
+      </c>
+      <c r="BM40" t="n">
+        <v>3.226495276345871</v>
+      </c>
+      <c r="BN40" t="n">
+        <v>3.46405534086639</v>
+      </c>
+      <c r="BO40" t="n">
+        <v>2.903483461716442</v>
+      </c>
+      <c r="BP40" t="n">
+        <v>1.854267264762022</v>
+      </c>
+      <c r="BQ40" t="n">
+        <v>0.4983746371463011</v>
+      </c>
+      <c r="BR40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>4</v>
+      </c>
+      <c r="B41" t="n">
+        <v>60</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1152.395833333333</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1152.395828513414</v>
+      </c>
+      <c r="G41" t="n">
+        <v>4.1825209324325e-09</v>
+      </c>
+      <c r="H41" t="n">
+        <v>24.87684607505798</v>
+      </c>
+      <c r="I41" t="n">
+        <v>600</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>13.20413414377076</v>
+      </c>
+      <c r="N41" t="n">
+        <v>13.64731070409568</v>
+      </c>
+      <c r="O41" t="n">
+        <v>14.39502839284668</v>
+      </c>
+      <c r="P41" t="n">
+        <v>14.70769163758868</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>14.47917754139388</v>
+      </c>
+      <c r="R41" t="n">
+        <v>11.98813251708912</v>
+      </c>
+      <c r="S41" t="n">
+        <v>9.857335211073794</v>
+      </c>
+      <c r="T41" t="n">
+        <v>11.92711133949038</v>
+      </c>
+      <c r="U41" t="n">
+        <v>13.16142695141954</v>
+      </c>
+      <c r="V41" t="n">
+        <v>13.96614872204771</v>
+      </c>
+      <c r="W41" t="n">
+        <v>14.42266924344836</v>
+      </c>
+      <c r="X41" t="n">
+        <v>14.43416204432724</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>12.13477570291715</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>10.04958184908295</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>11.83358878559851</v>
+      </c>
+      <c r="AB41" t="n">
+        <v>12.66260699577454</v>
+      </c>
+      <c r="AC41" t="n">
+        <v>13.68395340172063</v>
+      </c>
+      <c r="AD41" t="n">
+        <v>14.42330651831992</v>
+      </c>
+      <c r="AE41" t="n">
+        <v>14.56219709864665</v>
+      </c>
+      <c r="AF41" t="n">
+        <v>12.21457653453469</v>
+      </c>
+      <c r="AG41" t="n">
+        <v>10.06669482776361</v>
+      </c>
+      <c r="AH41" t="n">
+        <v>12.19050581517905</v>
+      </c>
+      <c r="AI41" t="n">
+        <v>13.41174783914677</v>
+      </c>
+      <c r="AJ41" t="n">
+        <v>14.23620472049324</v>
+      </c>
+      <c r="AK41" t="n">
+        <v>14.67326859739547</v>
+      </c>
+      <c r="AL41" t="n">
+        <v>14.89398459622751</v>
+      </c>
+      <c r="AM41" t="n">
+        <v>12.44242459092701</v>
+      </c>
+      <c r="AN41" t="n">
+        <v>10.21877944365803</v>
+      </c>
+      <c r="AO41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ41" t="n">
+        <v>2.09303439773183</v>
+      </c>
+      <c r="AR41" t="n">
+        <v>2.916440373835377</v>
+      </c>
+      <c r="AS41" t="n">
+        <v>3.294521630059289</v>
+      </c>
+      <c r="AT41" t="n">
+        <v>2.716931123688434</v>
+      </c>
+      <c r="AU41" t="n">
+        <v>1.782550319934487</v>
+      </c>
+      <c r="AV41" t="n">
+        <v>0.5074820405438616</v>
+      </c>
+      <c r="AW41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX41" t="n">
+        <v>2.521422992835885</v>
+      </c>
+      <c r="AY41" t="n">
+        <v>3.382749356284003</v>
+      </c>
+      <c r="AZ41" t="n">
+        <v>3.46907219847798</v>
+      </c>
+      <c r="BA41" t="n">
+        <v>2.928343665922319</v>
+      </c>
+      <c r="BB41" t="n">
+        <v>1.820531153960021</v>
+      </c>
+      <c r="BC41" t="n">
+        <v>0.473102009940926</v>
+      </c>
+      <c r="BD41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE41" t="n">
+        <v>2.491386626253388</v>
+      </c>
+      <c r="BF41" t="n">
+        <v>3.193913316005613</v>
+      </c>
+      <c r="BG41" t="n">
+        <v>3.482408533775299</v>
+      </c>
+      <c r="BH41" t="n">
+        <v>2.96289420296091</v>
+      </c>
+      <c r="BI41" t="n">
+        <v>1.758030628338735</v>
+      </c>
+      <c r="BJ41" t="n">
+        <v>0.4415535930675304</v>
+      </c>
+      <c r="BK41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL41" t="n">
+        <v>2.651244571085123</v>
+      </c>
+      <c r="BM41" t="n">
+        <v>3.396207056444647</v>
+      </c>
+      <c r="BN41" t="n">
+        <v>3.526294297719686</v>
+      </c>
+      <c r="BO41" t="n">
+        <v>3.088439204594904</v>
+      </c>
+      <c r="BP41" t="n">
+        <v>1.692862862151019</v>
+      </c>
+      <c r="BQ41" t="n">
+        <v>0.3589975220883374</v>
+      </c>
+      <c r="BR41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>------------------- Begin Heuristic -------------------</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" t="n">
+        <v>60</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1267.987499420073</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1267.987499418726</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.062462388325831e-12</v>
+      </c>
+      <c r="H43" t="n">
+        <v>12.372722864151</v>
+      </c>
+      <c r="I43" t="n">
+        <v>10</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>13.28275811107021</v>
+      </c>
+      <c r="N43" t="n">
+        <v>13.81060965544902</v>
+      </c>
+      <c r="O43" t="n">
+        <v>14.55365742178152</v>
+      </c>
+      <c r="P43" t="n">
+        <v>14.77060618523004</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>14.38134074517746</v>
+      </c>
+      <c r="R43" t="n">
+        <v>11.88571971760573</v>
+      </c>
+      <c r="S43" t="n">
+        <v>9.821482330215053</v>
+      </c>
+      <c r="T43" t="n">
+        <v>11.86631278448329</v>
+      </c>
+      <c r="U43" t="n">
+        <v>13.22751260397418</v>
+      </c>
+      <c r="V43" t="n">
+        <v>14.02631153041154</v>
+      </c>
+      <c r="W43" t="n">
+        <v>14.32299325255139</v>
+      </c>
+      <c r="X43" t="n">
+        <v>14.33247119568833</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>12.07993613564321</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>10.02584285972411</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>11.92367178916854</v>
+      </c>
+      <c r="AB43" t="n">
+        <v>12.74124552771992</v>
+      </c>
+      <c r="AC43" t="n">
+        <v>13.76251225297459</v>
+      </c>
+      <c r="AD43" t="n">
+        <v>14.24682102706906</v>
+      </c>
+      <c r="AE43" t="n">
+        <v>14.29642825735988</v>
+      </c>
+      <c r="AF43" t="n">
+        <v>11.96469215372369</v>
+      </c>
+      <c r="AG43" t="n">
+        <v>9.938288296738895</v>
+      </c>
+      <c r="AH43" t="n">
+        <v>11.98357186870942</v>
+      </c>
+      <c r="AI43" t="n">
+        <v>13.20807237605699</v>
+      </c>
+      <c r="AJ43" t="n">
+        <v>14.02852255104175</v>
+      </c>
+      <c r="AK43" t="n">
+        <v>14.38094077750022</v>
+      </c>
+      <c r="AL43" t="n">
+        <v>14.61949239273643</v>
+      </c>
+      <c r="AM43" t="n">
+        <v>12.24311890647004</v>
+      </c>
+      <c r="AN43" t="n">
+        <v>10.083861044767</v>
+      </c>
+      <c r="AO43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ43" t="n">
+        <v>2.213092271204963</v>
+      </c>
+      <c r="AR43" t="n">
+        <v>2.893591261925959</v>
+      </c>
+      <c r="AS43" t="n">
+        <v>3.215683212817568</v>
+      </c>
+      <c r="AT43" t="n">
+        <v>2.727359771582864</v>
+      </c>
+      <c r="AU43" t="n">
+        <v>1.761740755925019</v>
+      </c>
+      <c r="AV43" t="n">
+        <v>0.4886531246765014</v>
+      </c>
+      <c r="AW43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX43" t="n">
+        <v>2.572377524460233</v>
+      </c>
+      <c r="AY43" t="n">
+        <v>3.386774708318295</v>
+      </c>
+      <c r="AZ43" t="n">
+        <v>3.435353808647745</v>
+      </c>
+      <c r="BA43" t="n">
+        <v>2.879820212056619</v>
+      </c>
+      <c r="BB43" t="n">
+        <v>1.82393038228089</v>
+      </c>
+      <c r="BC43" t="n">
+        <v>0.4844724255751715</v>
+      </c>
+      <c r="BD43" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE43" t="n">
+        <v>2.548544627890144</v>
+      </c>
+      <c r="BF43" t="n">
+        <v>3.216703920750767</v>
+      </c>
+      <c r="BG43" t="n">
+        <v>3.338579605710165</v>
+      </c>
+      <c r="BH43" t="n">
+        <v>2.858106099465914</v>
+      </c>
+      <c r="BI43" t="n">
+        <v>1.767510174985133</v>
+      </c>
+      <c r="BJ43" t="n">
+        <v>0.4579661716264723</v>
+      </c>
+      <c r="BK43" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL43" t="n">
+        <v>2.510146064988316</v>
+      </c>
+      <c r="BM43" t="n">
+        <v>3.402480160072339</v>
+      </c>
+      <c r="BN43" t="n">
+        <v>3.562328745749125</v>
+      </c>
+      <c r="BO43" t="n">
+        <v>2.971616250229451</v>
+      </c>
+      <c r="BP43" t="n">
+        <v>1.704031428008238</v>
+      </c>
+      <c r="BQ43" t="n">
+        <v>0.39473695837384</v>
+      </c>
+      <c r="BR43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" t="n">
+        <v>60</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1267.987498759942</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1267.987498759942</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>13.00742101669312</v>
+      </c>
+      <c r="I44" t="n">
+        <v>10</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>13.24421204408409</v>
+      </c>
+      <c r="N44" t="n">
+        <v>13.68378625287019</v>
+      </c>
+      <c r="O44" t="n">
+        <v>14.45786247427242</v>
+      </c>
+      <c r="P44" t="n">
+        <v>14.86026985786329</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>14.68848390336043</v>
+      </c>
+      <c r="R44" t="n">
+        <v>12.17045784215429</v>
+      </c>
+      <c r="S44" t="n">
+        <v>9.99214093664099</v>
+      </c>
+      <c r="T44" t="n">
+        <v>11.91150533976702</v>
+      </c>
+      <c r="U44" t="n">
+        <v>13.28512550289438</v>
+      </c>
+      <c r="V44" t="n">
+        <v>14.0724233076524</v>
+      </c>
+      <c r="W44" t="n">
+        <v>14.27768469623976</v>
+      </c>
+      <c r="X44" t="n">
+        <v>14.29488701569552</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>11.99801339361114</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>10.0052418948126</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>11.82312797861839</v>
+      </c>
+      <c r="AB44" t="n">
+        <v>12.52876891925609</v>
+      </c>
+      <c r="AC44" t="n">
+        <v>13.51111282780435</v>
+      </c>
+      <c r="AD44" t="n">
+        <v>14.08236786724003</v>
+      </c>
+      <c r="AE44" t="n">
+        <v>14.15073367149934</v>
+      </c>
+      <c r="AF44" t="n">
+        <v>11.88202307731121</v>
+      </c>
+      <c r="AG44" t="n">
+        <v>9.819726952653744</v>
+      </c>
+      <c r="AH44" t="n">
+        <v>11.89034303463185</v>
+      </c>
+      <c r="AI44" t="n">
+        <v>13.18700171516948</v>
+      </c>
+      <c r="AJ44" t="n">
+        <v>14.06192026627433</v>
+      </c>
+      <c r="AK44" t="n">
+        <v>14.62234034975808</v>
+      </c>
+      <c r="AL44" t="n">
+        <v>14.92639081870649</v>
+      </c>
+      <c r="AM44" t="n">
+        <v>12.36794478988321</v>
+      </c>
+      <c r="AN44" t="n">
+        <v>10.18631885921948</v>
+      </c>
+      <c r="AO44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ44" t="n">
+        <v>2.168799656075856</v>
+      </c>
+      <c r="AR44" t="n">
+        <v>2.995322263150816</v>
+      </c>
+      <c r="AS44" t="n">
+        <v>3.332353256395845</v>
+      </c>
+      <c r="AT44" t="n">
+        <v>2.773495931075417</v>
+      </c>
+      <c r="AU44" t="n">
+        <v>1.758531506504851</v>
+      </c>
+      <c r="AV44" t="n">
+        <v>0.4715442576742492</v>
+      </c>
+      <c r="AW44" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX44" t="n">
+        <v>2.539925162688138</v>
+      </c>
+      <c r="AY44" t="n">
+        <v>3.387974525854152</v>
+      </c>
+      <c r="AZ44" t="n">
+        <v>3.460383596781832</v>
+      </c>
+      <c r="BA44" t="n">
+        <v>2.770973394158337</v>
+      </c>
+      <c r="BB44" t="n">
+        <v>1.815307321997275</v>
+      </c>
+      <c r="BC44" t="n">
+        <v>0.519698774642618</v>
+      </c>
+      <c r="BD44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE44" t="n">
+        <v>2.408862703169215</v>
+      </c>
+      <c r="BF44" t="n">
+        <v>3.064349504787724</v>
+      </c>
+      <c r="BG44" t="n">
+        <v>3.379756304652966</v>
+      </c>
+      <c r="BH44" t="n">
+        <v>2.899367711226899</v>
+      </c>
+      <c r="BI44" t="n">
+        <v>1.732082491076741</v>
+      </c>
+      <c r="BJ44" t="n">
+        <v>0.4404907670200998</v>
+      </c>
+      <c r="BK44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL44" t="n">
+        <v>2.66760701165064</v>
+      </c>
+      <c r="BM44" t="n">
+        <v>3.415473209065389</v>
+      </c>
+      <c r="BN44" t="n">
+        <v>3.501651514621576</v>
+      </c>
+      <c r="BO44" t="n">
+        <v>2.909694480657594</v>
+      </c>
+      <c r="BP44" t="n">
+        <v>1.75710978606323</v>
+      </c>
+      <c r="BQ44" t="n">
+        <v>0.4448445322554384</v>
+      </c>
+      <c r="BR44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4</v>
+      </c>
+      <c r="B45" t="n">
+        <v>60</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1253.608325026152</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1253.608325013861</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9.804789822892905e-12</v>
+      </c>
+      <c r="H45" t="n">
+        <v>18.80564999580383</v>
+      </c>
+      <c r="I45" t="n">
+        <v>10</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>13.06465502939268</v>
+      </c>
+      <c r="N45" t="n">
+        <v>13.72060727388059</v>
+      </c>
+      <c r="O45" t="n">
+        <v>14.38822164771619</v>
+      </c>
+      <c r="P45" t="n">
+        <v>14.64951421396679</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>14.45647386562628</v>
+      </c>
+      <c r="R45" t="n">
+        <v>12.01270037905369</v>
+      </c>
+      <c r="S45" t="n">
+        <v>9.909645020039839</v>
+      </c>
+      <c r="T45" t="n">
+        <v>12.05141956130963</v>
+      </c>
+      <c r="U45" t="n">
+        <v>13.14514752042842</v>
+      </c>
+      <c r="V45" t="n">
+        <v>13.92521355533944</v>
+      </c>
+      <c r="W45" t="n">
+        <v>14.46147289903581</v>
+      </c>
+      <c r="X45" t="n">
+        <v>14.41988916622038</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>12.10481324100714</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>10.05384434688477</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>11.73767889710938</v>
+      </c>
+      <c r="AB45" t="n">
+        <v>12.57175843034741</v>
+      </c>
+      <c r="AC45" t="n">
+        <v>13.46626997541981</v>
+      </c>
+      <c r="AD45" t="n">
+        <v>14.16360629392378</v>
+      </c>
+      <c r="AE45" t="n">
+        <v>14.31016093731113</v>
+      </c>
+      <c r="AF45" t="n">
+        <v>12.01304719969226</v>
+      </c>
+      <c r="AG45" t="n">
+        <v>9.945641696949577</v>
+      </c>
+      <c r="AH45" t="n">
+        <v>12.04908993224881</v>
+      </c>
+      <c r="AI45" t="n">
+        <v>13.36280112898558</v>
+      </c>
+      <c r="AJ45" t="n">
+        <v>14.11233255698316</v>
+      </c>
+      <c r="AK45" t="n">
+        <v>14.60251529363756</v>
+      </c>
+      <c r="AL45" t="n">
+        <v>14.55457899680351</v>
+      </c>
+      <c r="AM45" t="n">
+        <v>12.20176073070387</v>
+      </c>
+      <c r="AN45" t="n">
+        <v>10.12309883789147</v>
+      </c>
+      <c r="AO45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ45" t="n">
+        <v>2.081111845563803</v>
+      </c>
+      <c r="AR45" t="n">
+        <v>2.950428565667762</v>
+      </c>
+      <c r="AS45" t="n">
+        <v>3.199694871679041</v>
+      </c>
+      <c r="AT45" t="n">
+        <v>2.728748715120237</v>
+      </c>
+      <c r="AU45" t="n">
+        <v>1.819401517107379</v>
+      </c>
+      <c r="AV45" t="n">
+        <v>0.5032851453250387</v>
+      </c>
+      <c r="AW45" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX45" t="n">
+        <v>2.559164352733784</v>
+      </c>
+      <c r="AY45" t="n">
+        <v>3.400440842121335</v>
+      </c>
+      <c r="AZ45" t="n">
+        <v>3.402329346851425</v>
+      </c>
+      <c r="BA45" t="n">
+        <v>2.865703206442257</v>
+      </c>
+      <c r="BB45" t="n">
+        <v>1.811130661630575</v>
+      </c>
+      <c r="BC45" t="n">
+        <v>0.4704013427837972</v>
+      </c>
+      <c r="BD45" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE45" t="n">
+        <v>2.229787899942442</v>
+      </c>
+      <c r="BF45" t="n">
+        <v>3.073024120631665</v>
+      </c>
+      <c r="BG45" t="n">
+        <v>3.452224126932398</v>
+      </c>
+      <c r="BH45" t="n">
+        <v>3.036652886029625</v>
+      </c>
+      <c r="BI45" t="n">
+        <v>1.79757089517677</v>
+      </c>
+      <c r="BJ45" t="n">
+        <v>0.4388216959119142</v>
+      </c>
+      <c r="BK45" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL45" t="n">
+        <v>2.581688564990925</v>
+      </c>
+      <c r="BM45" t="n">
+        <v>3.400546444038388</v>
+      </c>
+      <c r="BN45" t="n">
+        <v>3.434447673842107</v>
+      </c>
+      <c r="BO45" t="n">
+        <v>2.920579952991958</v>
+      </c>
+      <c r="BP45" t="n">
+        <v>1.809211001368219</v>
+      </c>
+      <c r="BQ45" t="n">
+        <v>0.4673400431443981</v>
+      </c>
+      <c r="BR45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>4</v>
+      </c>
+      <c r="B46" t="n">
+        <v>60</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1253.608333333334</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1253.608328701471</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3.694824145508521e-09</v>
+      </c>
+      <c r="H46" t="n">
+        <v>16.74741005897522</v>
+      </c>
+      <c r="I46" t="n">
+        <v>10</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>13.06465502939268</v>
+      </c>
+      <c r="N46" t="n">
+        <v>13.72060727388059</v>
+      </c>
+      <c r="O46" t="n">
+        <v>14.38822164771619</v>
+      </c>
+      <c r="P46" t="n">
+        <v>14.6485671396833</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>14.46097593926975</v>
+      </c>
+      <c r="R46" t="n">
+        <v>12.00896403861225</v>
+      </c>
+      <c r="S46" t="n">
+        <v>9.9007613795095</v>
+      </c>
+      <c r="T46" t="n">
+        <v>12.04305671581905</v>
+      </c>
+      <c r="U46" t="n">
+        <v>13.1368509103418</v>
+      </c>
+      <c r="V46" t="n">
+        <v>13.91846169166459</v>
+      </c>
+      <c r="W46" t="n">
+        <v>14.45461080213492</v>
+      </c>
+      <c r="X46" t="n">
+        <v>14.40626840480447</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>12.10042340026424</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>10.05667212263751</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>11.74512943661266</v>
+      </c>
+      <c r="AB46" t="n">
+        <v>12.58057886837341</v>
+      </c>
+      <c r="AC46" t="n">
+        <v>13.47586253891125</v>
+      </c>
+      <c r="AD46" t="n">
+        <v>14.17245522132752</v>
+      </c>
+      <c r="AE46" t="n">
+        <v>14.30978464028104</v>
+      </c>
+      <c r="AF46" t="n">
+        <v>12.01837794016504</v>
+      </c>
+      <c r="AG46" t="n">
+        <v>9.958032312661219</v>
+      </c>
+      <c r="AH46" t="n">
+        <v>12.06195102684056</v>
+      </c>
+      <c r="AI46" t="n">
+        <v>13.37496858667169</v>
+      </c>
+      <c r="AJ46" t="n">
+        <v>14.12182002498749</v>
+      </c>
+      <c r="AK46" t="n">
+        <v>14.61452900666813</v>
+      </c>
+      <c r="AL46" t="n">
+        <v>14.56228851356756</v>
+      </c>
+      <c r="AM46" t="n">
+        <v>12.20124896622798</v>
+      </c>
+      <c r="AN46" t="n">
+        <v>10.11918432662592</v>
+      </c>
+      <c r="AO46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ46" t="n">
+        <v>2.081111845563803</v>
+      </c>
+      <c r="AR46" t="n">
+        <v>2.950428565667762</v>
+      </c>
+      <c r="AS46" t="n">
+        <v>3.199694871679041</v>
+      </c>
+      <c r="AT46" t="n">
+        <v>2.70624500290531</v>
+      </c>
+      <c r="AU46" t="n">
+        <v>1.81908999115144</v>
+      </c>
+      <c r="AV46" t="n">
+        <v>0.5105432098411676</v>
+      </c>
+      <c r="AW46" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX46" t="n">
+        <v>2.559164352733784</v>
+      </c>
+      <c r="AY46" t="n">
+        <v>3.400440842121335</v>
+      </c>
+      <c r="AZ46" t="n">
+        <v>3.402329346851425</v>
+      </c>
+      <c r="BA46" t="n">
+        <v>2.855218211891634</v>
+      </c>
+      <c r="BB46" t="n">
+        <v>1.823426845658747</v>
+      </c>
+      <c r="BC46" t="n">
+        <v>0.4823572576655229</v>
+      </c>
+      <c r="BD46" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE46" t="n">
+        <v>2.229787899942442</v>
+      </c>
+      <c r="BF46" t="n">
+        <v>3.073024120631665</v>
+      </c>
+      <c r="BG46" t="n">
+        <v>3.452224126932398</v>
+      </c>
+      <c r="BH46" t="n">
+        <v>3.048671603693929</v>
+      </c>
+      <c r="BI46" t="n">
+        <v>1.801750642464266</v>
+      </c>
+      <c r="BJ46" t="n">
+        <v>0.438181707518844</v>
+      </c>
+      <c r="BK46" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL46" t="n">
+        <v>2.581688564990925</v>
+      </c>
+      <c r="BM46" t="n">
+        <v>3.400546444038388</v>
+      </c>
+      <c r="BN46" t="n">
+        <v>3.434447673842107</v>
+      </c>
+      <c r="BO46" t="n">
+        <v>2.911258711993127</v>
+      </c>
+      <c r="BP46" t="n">
+        <v>1.804215173213408</v>
+      </c>
+      <c r="BQ46" t="n">
+        <v>0.4678886974176094</v>
+      </c>
+      <c r="BR46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>4</v>
+      </c>
+      <c r="B47" t="n">
+        <v>60</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1238.166666666667</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1238.166666666666</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>12.53124809265137</v>
+      </c>
+      <c r="I47" t="n">
+        <v>10</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>OPTIMAL</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>13.20103714501196</v>
+      </c>
+      <c r="N47" t="n">
+        <v>13.72485156226012</v>
+      </c>
+      <c r="O47" t="n">
+        <v>14.45742416889465</v>
+      </c>
+      <c r="P47" t="n">
+        <v>14.86738827364738</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>14.58095425620791</v>
+      </c>
+      <c r="R47" t="n">
+        <v>12.06577424646525</v>
+      </c>
+      <c r="S47" t="n">
+        <v>9.924466736831475</v>
+      </c>
+      <c r="T47" t="n">
+        <v>11.918902785544</v>
+      </c>
+      <c r="U47" t="n">
+        <v>13.1286471262773</v>
+      </c>
+      <c r="V47" t="n">
+        <v>13.90395780107393</v>
+      </c>
+      <c r="W47" t="n">
+        <v>14.28674221853868</v>
+      </c>
+      <c r="X47" t="n">
+        <v>14.40891414808336</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>11.99088258291762</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>9.855884775078049</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>11.68046790543767</v>
+      </c>
+      <c r="AB47" t="n">
+        <v>12.53379102697489</v>
+      </c>
+      <c r="AC47" t="n">
+        <v>13.50412507668399</v>
+      </c>
+      <c r="AD47" t="n">
+        <v>14.24305978128305</v>
+      </c>
+      <c r="AE47" t="n">
+        <v>14.42077118650924</v>
+      </c>
+      <c r="AF47" t="n">
+        <v>12.11257154698522</v>
+      </c>
+      <c r="AG47" t="n">
+        <v>10.03910533942733</v>
+      </c>
+      <c r="AH47" t="n">
+        <v>12.07578382086273</v>
+      </c>
+      <c r="AI47" t="n">
+        <v>13.28632893886657</v>
+      </c>
+      <c r="AJ47" t="n">
+        <v>14.06959157419851</v>
+      </c>
+      <c r="AK47" t="n">
+        <v>14.55993705391834</v>
+      </c>
+      <c r="AL47" t="n">
+        <v>14.83343387513662</v>
+      </c>
+      <c r="AM47" t="n">
+        <v>12.31653017211597</v>
+      </c>
+      <c r="AN47" t="n">
+        <v>10.06727646739249</v>
+      </c>
+      <c r="AO47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AP47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AQ47" t="n">
+        <v>2.154021259661389</v>
+      </c>
+      <c r="AR47" t="n">
+        <v>2.932154206018889</v>
+      </c>
+      <c r="AS47" t="n">
+        <v>3.252393905817269</v>
+      </c>
+      <c r="AT47" t="n">
+        <v>2.815695528540459</v>
+      </c>
+      <c r="AU47" t="n">
+        <v>1.787239633330324</v>
+      </c>
+      <c r="AV47" t="n">
+        <v>0.4785424276584107</v>
+      </c>
+      <c r="AW47" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX47" t="n">
+        <v>2.46915420248958</v>
+      </c>
+      <c r="AY47" t="n">
+        <v>3.357745112298522</v>
+      </c>
+      <c r="AZ47" t="n">
+        <v>3.501988667220193</v>
+      </c>
+      <c r="BA47" t="n">
+        <v>2.722026793264783</v>
+      </c>
+      <c r="BB47" t="n">
+        <v>1.736838223112741</v>
+      </c>
+      <c r="BC47" t="n">
+        <v>0.4846903873647174</v>
+      </c>
+      <c r="BD47" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE47" t="n">
+        <v>2.507176420356522</v>
+      </c>
+      <c r="BF47" t="n">
+        <v>3.182022909240017</v>
+      </c>
+      <c r="BG47" t="n">
+        <v>3.345686575486511</v>
+      </c>
+      <c r="BH47" t="n">
+        <v>3.062264201365363</v>
+      </c>
+      <c r="BI47" t="n">
+        <v>1.804106174086057</v>
+      </c>
+      <c r="BJ47" t="n">
+        <v>0.4155855178530763</v>
+      </c>
+      <c r="BK47" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL47" t="n">
+        <v>2.612890724540399</v>
+      </c>
+      <c r="BM47" t="n">
+        <v>3.34810618165018</v>
+      </c>
+      <c r="BN47" t="n">
+        <v>3.478574794370882</v>
+      </c>
+      <c r="BO47" t="n">
+        <v>2.917776480245807</v>
+      </c>
+      <c r="BP47" t="n">
+        <v>1.72084294901166</v>
+      </c>
+      <c r="BQ47" t="n">
+        <v>0.4103748364425409</v>
+      </c>
+      <c r="BR47" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>